<commit_message>
Added View Event code changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/jms/qa/testdata/JMSTestData.xlsx
+++ b/src/main/java/com/jms/qa/testdata/JMSTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C754CBD7-93A2-4F54-B613-2AD190EC2C90}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6B47BC98-39E4-47E2-A9F3-FA74DF80CDD7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16605" windowHeight="5895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JurorDetails" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="EventDetails2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O17"/>
+  <oleSize ref="A1:N17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,22 +100,22 @@
     <t>12345B</t>
   </si>
   <si>
-    <t>AutoCreate Event1</t>
-  </si>
-  <si>
-    <t>AutoCreate Event2</t>
-  </si>
-  <si>
     <t>Jurado</t>
   </si>
   <si>
     <t>12345C</t>
   </si>
   <si>
-    <t>10/22/2025</t>
-  </si>
-  <si>
-    <t>10/23/2025</t>
+    <t>CreateAutoEvent</t>
+  </si>
+  <si>
+    <t>10/29/2025</t>
+  </si>
+  <si>
+    <t>10/30/2025</t>
+  </si>
+  <si>
+    <t>CreateAuto Event2</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,10 +668,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -680,10 +680,10 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
@@ -694,10 +694,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -706,7 +706,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>

</xml_diff>